<commit_message>
fewshot frame args extraction
</commit_message>
<xml_diff>
--- a/Communication on Progress Questionnaire (French).xlsx
+++ b/Communication on Progress Questionnaire (French).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unistra\Unistra\Recherche\RAGbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE116E8-BF86-48CB-8F6E-FBD99681F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC966DB-CD59-4F5B-B1A4-D2784965879D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4682,6 +4682,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4689,7 +4692,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4709,11 +4712,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4725,9 +4725,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4747,6 +4744,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5793,8 +5793,8 @@
       <c r="B50" s="11"/>
     </row>
     <row r="51" spans="2:11" ht="64.8">
-      <c r="B51" s="97"/>
-      <c r="C51" s="99" t="s">
+      <c r="B51" s="98"/>
+      <c r="C51" s="100" t="s">
         <v>38</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -5811,8 +5811,8 @@
       </c>
     </row>
     <row r="52" spans="2:11" ht="130.19999999999999" thickBot="1">
-      <c r="B52" s="98"/>
-      <c r="C52" s="100"/>
+      <c r="B52" s="99"/>
+      <c r="C52" s="101"/>
       <c r="D52" s="1" t="s">
         <v>43</v>
       </c>
@@ -5937,8 +5937,8 @@
       <c r="B64" s="11"/>
     </row>
     <row r="65" spans="2:11" ht="64.8">
-      <c r="B65" s="97"/>
-      <c r="C65" s="99" t="s">
+      <c r="B65" s="98"/>
+      <c r="C65" s="100" t="s">
         <v>49</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -5955,8 +5955,8 @@
       </c>
     </row>
     <row r="66" spans="2:11" ht="216.6" thickBot="1">
-      <c r="B66" s="98"/>
-      <c r="C66" s="100"/>
+      <c r="B66" s="99"/>
+      <c r="C66" s="101"/>
       <c r="D66" s="1" t="s">
         <v>54</v>
       </c>
@@ -6086,13 +6086,13 @@
       <c r="B78" s="11"/>
     </row>
     <row r="79" spans="2:11" ht="140.4">
-      <c r="B79" s="101" t="s">
+      <c r="B79" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="C79" s="94" t="s">
+      <c r="C79" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="D79" s="94" t="s">
+      <c r="D79" s="95" t="s">
         <v>63</v>
       </c>
       <c r="E79" s="2" t="s">
@@ -6107,9 +6107,9 @@
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="2:11" ht="32.4">
-      <c r="B80" s="101"/>
-      <c r="C80" s="94"/>
-      <c r="D80" s="94"/>
+      <c r="B80" s="102"/>
+      <c r="C80" s="95"/>
+      <c r="D80" s="95"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2" t="s">
         <v>67</v>
@@ -6120,9 +6120,9 @@
       <c r="H80" s="2"/>
     </row>
     <row r="81" spans="2:8" ht="11.4" thickBot="1">
-      <c r="B81" s="102"/>
-      <c r="C81" s="95"/>
-      <c r="D81" s="95"/>
+      <c r="B81" s="103"/>
+      <c r="C81" s="96"/>
+      <c r="D81" s="96"/>
       <c r="E81" s="25"/>
       <c r="F81" s="25"/>
       <c r="G81" s="25"/>
@@ -6224,14 +6224,14 @@
       <c r="B89" s="3"/>
     </row>
     <row r="90" spans="2:8">
-      <c r="B90" s="96" t="s">
+      <c r="B90" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="C90" s="96"/>
-      <c r="D90" s="96"/>
-      <c r="E90" s="96"/>
-      <c r="F90" s="96"/>
-      <c r="G90" s="96"/>
+      <c r="C90" s="104"/>
+      <c r="D90" s="104"/>
+      <c r="E90" s="104"/>
+      <c r="F90" s="104"/>
+      <c r="G90" s="104"/>
     </row>
     <row r="91" spans="2:8">
       <c r="B91" s="24" t="s">
@@ -6243,37 +6243,37 @@
     </row>
     <row r="93" spans="2:8">
       <c r="B93" s="8"/>
-      <c r="C93" s="94" t="s">
+      <c r="C93" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="D93" s="94" t="s">
+      <c r="D93" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="E93" s="94"/>
-      <c r="F93" s="94"/>
+      <c r="E93" s="95"/>
+      <c r="F93" s="95"/>
     </row>
     <row r="94" spans="2:8">
       <c r="B94" s="8"/>
-      <c r="C94" s="94"/>
-      <c r="D94" s="94"/>
-      <c r="E94" s="94"/>
-      <c r="F94" s="94"/>
+      <c r="C94" s="95"/>
+      <c r="D94" s="95"/>
+      <c r="E94" s="95"/>
+      <c r="F94" s="95"/>
     </row>
     <row r="95" spans="2:8">
       <c r="B95" s="8"/>
-      <c r="C95" s="94"/>
-      <c r="D95" s="94"/>
-      <c r="E95" s="94"/>
-      <c r="F95" s="94"/>
+      <c r="C95" s="95"/>
+      <c r="D95" s="95"/>
+      <c r="E95" s="95"/>
+      <c r="F95" s="95"/>
     </row>
     <row r="96" spans="2:8" ht="22.2" thickBot="1">
       <c r="B96" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C96" s="95"/>
-      <c r="D96" s="95"/>
-      <c r="E96" s="94"/>
-      <c r="F96" s="94"/>
+      <c r="C96" s="96"/>
+      <c r="D96" s="96"/>
+      <c r="E96" s="95"/>
+      <c r="F96" s="95"/>
     </row>
     <row r="97" spans="2:7" ht="32.4">
       <c r="B97" s="5" t="s">
@@ -6339,14 +6339,14 @@
       <c r="B103" s="11"/>
     </row>
     <row r="104" spans="2:7">
-      <c r="B104" s="96" t="s">
+      <c r="B104" s="104" t="s">
         <v>75</v>
       </c>
-      <c r="C104" s="96"/>
-      <c r="D104" s="96"/>
-      <c r="E104" s="96"/>
-      <c r="F104" s="96"/>
-      <c r="G104" s="96"/>
+      <c r="C104" s="104"/>
+      <c r="D104" s="104"/>
+      <c r="E104" s="104"/>
+      <c r="F104" s="104"/>
+      <c r="G104" s="104"/>
     </row>
     <row r="105" spans="2:7">
       <c r="B105" s="23" t="s">
@@ -6363,10 +6363,10 @@
     </row>
     <row r="108" spans="2:7" ht="140.4">
       <c r="B108" s="8"/>
-      <c r="C108" s="94" t="s">
+      <c r="C108" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="D108" s="94" t="s">
+      <c r="D108" s="95" t="s">
         <v>63</v>
       </c>
       <c r="E108" s="2" t="s">
@@ -6381,8 +6381,8 @@
     </row>
     <row r="109" spans="2:7" ht="32.4">
       <c r="B109" s="8"/>
-      <c r="C109" s="94"/>
-      <c r="D109" s="94"/>
+      <c r="C109" s="95"/>
+      <c r="D109" s="95"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2" t="s">
         <v>77</v>
@@ -6395,8 +6395,8 @@
       <c r="B110" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C110" s="95"/>
-      <c r="D110" s="95"/>
+      <c r="C110" s="96"/>
+      <c r="D110" s="96"/>
       <c r="E110" s="25"/>
       <c r="F110" s="25"/>
       <c r="G110" s="25"/>
@@ -6493,15 +6493,15 @@
       <c r="B117" s="11"/>
     </row>
     <row r="118" spans="2:8">
-      <c r="B118" s="104" t="s">
+      <c r="B118" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="C118" s="104"/>
-      <c r="D118" s="104"/>
-      <c r="E118" s="104"/>
-      <c r="F118" s="104"/>
-      <c r="G118" s="104"/>
-      <c r="H118" s="104"/>
+      <c r="C118" s="97"/>
+      <c r="D118" s="97"/>
+      <c r="E118" s="97"/>
+      <c r="F118" s="97"/>
+      <c r="G118" s="97"/>
+      <c r="H118" s="97"/>
     </row>
     <row r="119" spans="2:8">
       <c r="B119" s="23" t="s">
@@ -6518,29 +6518,29 @@
     </row>
     <row r="122" spans="2:8">
       <c r="B122" s="8"/>
-      <c r="C122" s="94" t="s">
+      <c r="C122" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="D122" s="94" t="s">
+      <c r="D122" s="95" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="123" spans="2:8">
       <c r="B123" s="8"/>
-      <c r="C123" s="94"/>
-      <c r="D123" s="94"/>
+      <c r="C123" s="95"/>
+      <c r="D123" s="95"/>
     </row>
     <row r="124" spans="2:8">
       <c r="B124" s="8"/>
-      <c r="C124" s="94"/>
-      <c r="D124" s="94"/>
+      <c r="C124" s="95"/>
+      <c r="D124" s="95"/>
     </row>
     <row r="125" spans="2:8" ht="22.2" thickBot="1">
       <c r="B125" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C125" s="95"/>
-      <c r="D125" s="95"/>
+      <c r="C125" s="96"/>
+      <c r="D125" s="96"/>
     </row>
     <row r="126" spans="2:8" ht="32.4">
       <c r="B126" s="5" t="s">
@@ -6606,17 +6606,17 @@
       </c>
     </row>
     <row r="135" spans="2:10">
-      <c r="B135" s="103" t="s">
+      <c r="B135" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="C135" s="103"/>
-      <c r="D135" s="103"/>
-      <c r="E135" s="103"/>
-      <c r="F135" s="103"/>
-      <c r="G135" s="103"/>
-      <c r="H135" s="103"/>
-      <c r="I135" s="103"/>
-      <c r="J135" s="103"/>
+      <c r="C135" s="94"/>
+      <c r="D135" s="94"/>
+      <c r="E135" s="94"/>
+      <c r="F135" s="94"/>
+      <c r="G135" s="94"/>
+      <c r="H135" s="94"/>
+      <c r="I135" s="94"/>
+      <c r="J135" s="94"/>
     </row>
     <row r="136" spans="2:10">
       <c r="B136" s="23" t="s">
@@ -7308,6 +7308,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="B90:G90"/>
+    <mergeCell ref="B104:G104"/>
+    <mergeCell ref="C108:C110"/>
+    <mergeCell ref="D108:D110"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="B79:B81"/>
     <mergeCell ref="B135:J135"/>
     <mergeCell ref="C122:C125"/>
     <mergeCell ref="D122:D125"/>
@@ -7316,17 +7327,6 @@
     <mergeCell ref="B118:H118"/>
     <mergeCell ref="E93:E96"/>
     <mergeCell ref="F93:F96"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="B90:G90"/>
-    <mergeCell ref="B104:G104"/>
-    <mergeCell ref="C108:C110"/>
-    <mergeCell ref="D108:D110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7507,21 +7507,21 @@
       </c>
     </row>
     <row r="30" spans="2:14" ht="28.2" customHeight="1">
-      <c r="B30" s="104" t="s">
+      <c r="B30" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="104"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="104"/>
-      <c r="F30" s="104"/>
-      <c r="G30" s="104"/>
-      <c r="H30" s="104"/>
-      <c r="I30" s="104"/>
-      <c r="J30" s="104"/>
-      <c r="K30" s="104"/>
-      <c r="L30" s="104"/>
-      <c r="M30" s="104"/>
-      <c r="N30" s="104"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="97"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="97"/>
+      <c r="I30" s="97"/>
+      <c r="J30" s="97"/>
+      <c r="K30" s="97"/>
+      <c r="L30" s="97"/>
+      <c r="M30" s="97"/>
+      <c r="N30" s="97"/>
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="23" t="s">
@@ -7538,42 +7538,42 @@
     </row>
     <row r="34" spans="2:13">
       <c r="B34" s="8"/>
-      <c r="C34" s="94" t="s">
+      <c r="C34" s="95" t="s">
         <v>164</v>
       </c>
-      <c r="D34" s="94" t="s">
+      <c r="D34" s="95" t="s">
         <v>165</v>
       </c>
-      <c r="E34" s="94" t="s">
+      <c r="E34" s="95" t="s">
         <v>166</v>
       </c>
-      <c r="F34" s="94" t="s">
+      <c r="F34" s="95" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="8"/>
-      <c r="C35" s="94"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="94"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="95"/>
     </row>
     <row r="36" spans="2:13">
       <c r="B36" s="29"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
-      <c r="E36" s="94"/>
-      <c r="F36" s="94"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
       <c r="M36" s="22"/>
     </row>
     <row r="37" spans="2:13" ht="43.8" thickBot="1">
       <c r="B37" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95"/>
+      <c r="C37" s="96"/>
+      <c r="D37" s="96"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="96"/>
     </row>
     <row r="38" spans="2:13" ht="21.6">
       <c r="B38" s="5" t="s">
@@ -7713,65 +7713,65 @@
     </row>
     <row r="52" spans="2:13">
       <c r="B52" s="8"/>
-      <c r="C52" s="94" t="s">
+      <c r="C52" s="95" t="s">
         <v>180</v>
       </c>
-      <c r="D52" s="94" t="s">
+      <c r="D52" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="E52" s="94" t="s">
+      <c r="E52" s="95" t="s">
         <v>182</v>
       </c>
-      <c r="F52" s="94" t="s">
+      <c r="F52" s="95" t="s">
         <v>183</v>
       </c>
-      <c r="G52" s="94" t="s">
+      <c r="G52" s="95" t="s">
         <v>184</v>
       </c>
-      <c r="H52" s="94" t="s">
+      <c r="H52" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="I52" s="94" t="s">
+      <c r="I52" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="J52" s="94" t="s">
+      <c r="J52" s="95" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="53" spans="2:13">
       <c r="B53" s="8"/>
-      <c r="C53" s="94"/>
-      <c r="D53" s="94"/>
-      <c r="E53" s="94"/>
-      <c r="F53" s="94"/>
-      <c r="G53" s="94"/>
-      <c r="H53" s="94"/>
-      <c r="I53" s="94"/>
-      <c r="J53" s="94"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="95"/>
+      <c r="F53" s="95"/>
+      <c r="G53" s="95"/>
+      <c r="H53" s="95"/>
+      <c r="I53" s="95"/>
+      <c r="J53" s="95"/>
     </row>
     <row r="54" spans="2:13">
       <c r="B54" s="8"/>
-      <c r="C54" s="94"/>
-      <c r="D54" s="94"/>
-      <c r="E54" s="94"/>
-      <c r="F54" s="94"/>
-      <c r="G54" s="94"/>
-      <c r="H54" s="94"/>
-      <c r="I54" s="94"/>
-      <c r="J54" s="94"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="95"/>
+      <c r="H54" s="95"/>
+      <c r="I54" s="95"/>
+      <c r="J54" s="95"/>
     </row>
     <row r="55" spans="2:13" ht="43.8" thickBot="1">
       <c r="B55" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="C55" s="95"/>
-      <c r="D55" s="95"/>
-      <c r="E55" s="95"/>
-      <c r="F55" s="95"/>
-      <c r="G55" s="95"/>
-      <c r="H55" s="95"/>
-      <c r="I55" s="95"/>
-      <c r="J55" s="95"/>
+      <c r="C55" s="96"/>
+      <c r="D55" s="96"/>
+      <c r="E55" s="96"/>
+      <c r="F55" s="96"/>
+      <c r="G55" s="96"/>
+      <c r="H55" s="96"/>
+      <c r="I55" s="96"/>
+      <c r="J55" s="96"/>
     </row>
     <row r="56" spans="2:13" ht="21.6">
       <c r="B56" s="5" t="s">
@@ -7965,16 +7965,16 @@
       </c>
     </row>
     <row r="66" spans="2:12" ht="36" customHeight="1">
-      <c r="B66" s="104" t="s">
+      <c r="B66" s="97" t="s">
         <v>190</v>
       </c>
-      <c r="C66" s="104"/>
-      <c r="D66" s="104"/>
-      <c r="E66" s="104"/>
-      <c r="F66" s="104"/>
-      <c r="G66" s="104"/>
-      <c r="H66" s="104"/>
-      <c r="I66" s="104"/>
+      <c r="C66" s="97"/>
+      <c r="D66" s="97"/>
+      <c r="E66" s="97"/>
+      <c r="F66" s="97"/>
+      <c r="G66" s="97"/>
+      <c r="H66" s="97"/>
+      <c r="I66" s="97"/>
     </row>
     <row r="67" spans="2:12">
       <c r="B67" s="23" t="s">
@@ -7999,53 +7999,53 @@
     </row>
     <row r="72" spans="2:12" ht="10.199999999999999" customHeight="1">
       <c r="B72" s="8"/>
-      <c r="C72" s="94" t="s">
+      <c r="C72" s="95" t="s">
         <v>193</v>
       </c>
-      <c r="D72" s="94" t="s">
+      <c r="D72" s="95" t="s">
         <v>194</v>
       </c>
-      <c r="E72" s="94" t="s">
+      <c r="E72" s="95" t="s">
         <v>195</v>
       </c>
-      <c r="F72" s="94" t="s">
+      <c r="F72" s="95" t="s">
         <v>196</v>
       </c>
-      <c r="G72" s="94" t="s">
+      <c r="G72" s="95" t="s">
         <v>197</v>
       </c>
-      <c r="H72" s="94" t="s">
+      <c r="H72" s="95" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="73" spans="2:12">
       <c r="B73" s="8"/>
-      <c r="C73" s="94"/>
-      <c r="D73" s="94"/>
-      <c r="E73" s="94"/>
-      <c r="F73" s="94"/>
-      <c r="G73" s="94"/>
-      <c r="H73" s="94"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="95"/>
+      <c r="E73" s="95"/>
+      <c r="F73" s="95"/>
+      <c r="G73" s="95"/>
+      <c r="H73" s="95"/>
     </row>
     <row r="74" spans="2:12">
       <c r="B74" s="8"/>
-      <c r="C74" s="94"/>
-      <c r="D74" s="94"/>
-      <c r="E74" s="94"/>
-      <c r="F74" s="94"/>
-      <c r="G74" s="94"/>
-      <c r="H74" s="94"/>
+      <c r="C74" s="95"/>
+      <c r="D74" s="95"/>
+      <c r="E74" s="95"/>
+      <c r="F74" s="95"/>
+      <c r="G74" s="95"/>
+      <c r="H74" s="95"/>
     </row>
     <row r="75" spans="2:12" ht="43.8" thickBot="1">
       <c r="B75" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="C75" s="95"/>
-      <c r="D75" s="95"/>
-      <c r="E75" s="95"/>
-      <c r="F75" s="95"/>
-      <c r="G75" s="95"/>
-      <c r="H75" s="95"/>
+      <c r="C75" s="96"/>
+      <c r="D75" s="96"/>
+      <c r="E75" s="96"/>
+      <c r="F75" s="96"/>
+      <c r="G75" s="96"/>
+      <c r="H75" s="96"/>
     </row>
     <row r="76" spans="2:12" ht="21.6">
       <c r="B76" s="5" t="s">
@@ -8198,16 +8198,16 @@
       <c r="B85" s="11"/>
     </row>
     <row r="86" spans="2:9" ht="22.2" customHeight="1">
-      <c r="B86" s="104" t="s">
+      <c r="B86" s="97" t="s">
         <v>199</v>
       </c>
-      <c r="C86" s="104"/>
-      <c r="D86" s="104"/>
-      <c r="E86" s="104"/>
-      <c r="F86" s="104"/>
-      <c r="G86" s="104"/>
-      <c r="H86" s="104"/>
-      <c r="I86" s="104"/>
+      <c r="C86" s="97"/>
+      <c r="D86" s="97"/>
+      <c r="E86" s="97"/>
+      <c r="F86" s="97"/>
+      <c r="G86" s="97"/>
+      <c r="H86" s="97"/>
+      <c r="I86" s="97"/>
     </row>
     <row r="87" spans="2:9">
       <c r="B87" s="23" t="s">
@@ -8224,59 +8224,59 @@
     </row>
     <row r="90" spans="2:9" ht="71.400000000000006" customHeight="1">
       <c r="B90" s="8"/>
-      <c r="C90" s="94" t="s">
+      <c r="C90" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="D90" s="94" t="s">
+      <c r="D90" s="95" t="s">
         <v>202</v>
       </c>
-      <c r="E90" s="94" t="s">
+      <c r="E90" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="F90" s="94" t="s">
+      <c r="F90" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="G90" s="94" t="s">
+      <c r="G90" s="95" t="s">
         <v>205</v>
       </c>
-      <c r="H90" s="94" t="s">
+      <c r="H90" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="I90" s="94" t="s">
+      <c r="I90" s="95" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="91" spans="2:9">
       <c r="B91" s="8"/>
-      <c r="C91" s="94"/>
-      <c r="D91" s="94"/>
-      <c r="E91" s="94"/>
-      <c r="F91" s="94"/>
-      <c r="G91" s="94"/>
-      <c r="H91" s="94"/>
-      <c r="I91" s="94"/>
+      <c r="C91" s="95"/>
+      <c r="D91" s="95"/>
+      <c r="E91" s="95"/>
+      <c r="F91" s="95"/>
+      <c r="G91" s="95"/>
+      <c r="H91" s="95"/>
+      <c r="I91" s="95"/>
     </row>
     <row r="92" spans="2:9">
       <c r="B92" s="8"/>
-      <c r="C92" s="94"/>
-      <c r="D92" s="94"/>
-      <c r="E92" s="94"/>
-      <c r="F92" s="94"/>
-      <c r="G92" s="94"/>
-      <c r="H92" s="94"/>
-      <c r="I92" s="94"/>
+      <c r="C92" s="95"/>
+      <c r="D92" s="95"/>
+      <c r="E92" s="95"/>
+      <c r="F92" s="95"/>
+      <c r="G92" s="95"/>
+      <c r="H92" s="95"/>
+      <c r="I92" s="95"/>
     </row>
     <row r="93" spans="2:9" ht="9" customHeight="1" thickBot="1">
       <c r="B93" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="C93" s="95"/>
-      <c r="D93" s="95"/>
-      <c r="E93" s="95"/>
-      <c r="F93" s="95"/>
-      <c r="G93" s="95"/>
+      <c r="C93" s="96"/>
+      <c r="D93" s="96"/>
+      <c r="E93" s="96"/>
+      <c r="F93" s="96"/>
+      <c r="G93" s="96"/>
       <c r="H93" s="25"/>
-      <c r="I93" s="95"/>
+      <c r="I93" s="96"/>
     </row>
     <row r="94" spans="2:9" ht="21.6">
       <c r="B94" s="5" t="s">
@@ -8465,59 +8465,59 @@
     </row>
     <row r="107" spans="2:9">
       <c r="B107" s="8"/>
-      <c r="C107" s="94" t="s">
+      <c r="C107" s="95" t="s">
         <v>209</v>
       </c>
-      <c r="D107" s="94" t="s">
+      <c r="D107" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="E107" s="94" t="s">
+      <c r="E107" s="95" t="s">
         <v>211</v>
       </c>
-      <c r="F107" s="94" t="s">
+      <c r="F107" s="95" t="s">
         <v>212</v>
       </c>
-      <c r="G107" s="94" t="s">
+      <c r="G107" s="95" t="s">
         <v>213</v>
       </c>
-      <c r="H107" s="94" t="s">
+      <c r="H107" s="95" t="s">
         <v>214</v>
       </c>
-      <c r="I107" s="94" t="s">
+      <c r="I107" s="95" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="108" spans="2:9">
       <c r="B108" s="8"/>
-      <c r="C108" s="94"/>
-      <c r="D108" s="94"/>
-      <c r="E108" s="94"/>
-      <c r="F108" s="94"/>
-      <c r="G108" s="94"/>
-      <c r="H108" s="94"/>
-      <c r="I108" s="94"/>
+      <c r="C108" s="95"/>
+      <c r="D108" s="95"/>
+      <c r="E108" s="95"/>
+      <c r="F108" s="95"/>
+      <c r="G108" s="95"/>
+      <c r="H108" s="95"/>
+      <c r="I108" s="95"/>
     </row>
     <row r="109" spans="2:9">
       <c r="B109" s="8"/>
-      <c r="C109" s="94"/>
-      <c r="D109" s="94"/>
-      <c r="E109" s="94"/>
-      <c r="F109" s="94"/>
-      <c r="G109" s="94"/>
-      <c r="H109" s="94"/>
-      <c r="I109" s="94"/>
+      <c r="C109" s="95"/>
+      <c r="D109" s="95"/>
+      <c r="E109" s="95"/>
+      <c r="F109" s="95"/>
+      <c r="G109" s="95"/>
+      <c r="H109" s="95"/>
+      <c r="I109" s="95"/>
     </row>
     <row r="110" spans="2:9" ht="43.8" thickBot="1">
       <c r="B110" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="C110" s="95"/>
-      <c r="D110" s="95"/>
-      <c r="E110" s="95"/>
-      <c r="F110" s="95"/>
-      <c r="G110" s="95"/>
-      <c r="H110" s="95"/>
-      <c r="I110" s="95"/>
+      <c r="C110" s="96"/>
+      <c r="D110" s="96"/>
+      <c r="E110" s="96"/>
+      <c r="F110" s="96"/>
+      <c r="G110" s="96"/>
+      <c r="H110" s="96"/>
+      <c r="I110" s="96"/>
     </row>
     <row r="111" spans="2:9" ht="21.6">
       <c r="B111" s="5" t="s">
@@ -8687,16 +8687,16 @@
       <c r="B120" s="11"/>
     </row>
     <row r="121" spans="2:9" ht="25.2" customHeight="1">
-      <c r="B121" s="104" t="s">
+      <c r="B121" s="97" t="s">
         <v>216</v>
       </c>
-      <c r="C121" s="104"/>
-      <c r="D121" s="104"/>
-      <c r="E121" s="104"/>
-      <c r="F121" s="104"/>
-      <c r="G121" s="104"/>
-      <c r="H121" s="104"/>
-      <c r="I121" s="104"/>
+      <c r="C121" s="97"/>
+      <c r="D121" s="97"/>
+      <c r="E121" s="97"/>
+      <c r="F121" s="97"/>
+      <c r="G121" s="97"/>
+      <c r="H121" s="97"/>
+      <c r="I121" s="97"/>
     </row>
     <row r="122" spans="2:9">
       <c r="B122" s="23" t="s">
@@ -8874,16 +8874,16 @@
       </c>
     </row>
     <row r="138" spans="2:9" ht="23.4" customHeight="1">
-      <c r="B138" s="104" t="s">
+      <c r="B138" s="97" t="s">
         <v>223</v>
       </c>
-      <c r="C138" s="104"/>
-      <c r="D138" s="104"/>
-      <c r="E138" s="104"/>
-      <c r="F138" s="104"/>
-      <c r="G138" s="104"/>
-      <c r="H138" s="104"/>
-      <c r="I138" s="104"/>
+      <c r="C138" s="97"/>
+      <c r="D138" s="97"/>
+      <c r="E138" s="97"/>
+      <c r="F138" s="97"/>
+      <c r="G138" s="97"/>
+      <c r="H138" s="97"/>
+      <c r="I138" s="97"/>
     </row>
     <row r="139" spans="2:9">
       <c r="B139" s="23" t="s">
@@ -9058,6 +9058,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="F90:F93"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="B86:I86"/>
+    <mergeCell ref="G90:G93"/>
+    <mergeCell ref="H90:H92"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="H72:H75"/>
+    <mergeCell ref="H52:H55"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="D90:D93"/>
+    <mergeCell ref="E90:E93"/>
+    <mergeCell ref="G107:G110"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
     <mergeCell ref="H107:H110"/>
     <mergeCell ref="B66:I66"/>
     <mergeCell ref="B121:I121"/>
@@ -9074,29 +9097,6 @@
     <mergeCell ref="D107:D110"/>
     <mergeCell ref="E107:E110"/>
     <mergeCell ref="F107:F110"/>
-    <mergeCell ref="D90:D93"/>
-    <mergeCell ref="E90:E93"/>
-    <mergeCell ref="G107:G110"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="F90:F93"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="B86:I86"/>
-    <mergeCell ref="G90:G93"/>
-    <mergeCell ref="H90:H92"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="H72:H75"/>
-    <mergeCell ref="H52:H55"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="F34:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9164,39 +9164,39 @@
     </row>
     <row r="9" spans="1:13" ht="91.95" customHeight="1">
       <c r="B9" s="8"/>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="95" t="s">
         <v>236</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="95" t="s">
         <v>237</v>
       </c>
-      <c r="E9" s="94" t="s">
+      <c r="E9" s="95" t="s">
         <v>238</v>
       </c>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="95" t="s">
         <v>239</v>
       </c>
-      <c r="G9" s="94" t="s">
+      <c r="G9" s="95" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="8"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
     </row>
     <row r="11" spans="1:13" ht="22.2" thickBot="1">
       <c r="B11" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
       <c r="F11" s="25"/>
-      <c r="G11" s="95"/>
+      <c r="G11" s="96"/>
     </row>
     <row r="12" spans="1:13" ht="75.599999999999994">
       <c r="B12" s="5" t="s">
@@ -9364,64 +9364,64 @@
     </row>
     <row r="29" spans="2:14" ht="102" customHeight="1">
       <c r="B29" s="8"/>
-      <c r="C29" s="94" t="s">
+      <c r="C29" s="95" t="s">
         <v>253</v>
       </c>
-      <c r="D29" s="94" t="s">
+      <c r="D29" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="E29" s="94" t="s">
+      <c r="E29" s="95" t="s">
         <v>254</v>
       </c>
-      <c r="F29" s="94" t="s">
+      <c r="F29" s="95" t="s">
         <v>183</v>
       </c>
-      <c r="G29" s="94" t="s">
+      <c r="G29" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="H29" s="94" t="s">
+      <c r="H29" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="I29" s="94" t="s">
+      <c r="I29" s="95" t="s">
         <v>257</v>
       </c>
-      <c r="J29" s="94" t="s">
+      <c r="J29" s="95" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="8"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="95"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="95"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="8"/>
-      <c r="C31" s="94"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="94"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="94"/>
-      <c r="I31" s="94"/>
-      <c r="J31" s="94"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="95"/>
+      <c r="F31" s="95"/>
+      <c r="G31" s="95"/>
+      <c r="H31" s="95"/>
+      <c r="I31" s="95"/>
+      <c r="J31" s="95"/>
     </row>
     <row r="32" spans="2:14" ht="22.2" thickBot="1">
       <c r="B32" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C32" s="95"/>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="95"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="96"/>
+      <c r="I32" s="96"/>
       <c r="J32" s="25"/>
     </row>
     <row r="33" spans="2:13" ht="75.599999999999994">
@@ -10196,49 +10196,49 @@
     </row>
     <row r="99" spans="2:9">
       <c r="B99" s="8"/>
-      <c r="C99" s="94" t="s">
+      <c r="C99" s="95" t="s">
         <v>282</v>
       </c>
-      <c r="D99" s="94" t="s">
+      <c r="D99" s="95" t="s">
         <v>283</v>
       </c>
-      <c r="E99" s="94" t="s">
+      <c r="E99" s="95" t="s">
         <v>284</v>
       </c>
-      <c r="F99" s="94" t="s">
+      <c r="F99" s="95" t="s">
         <v>212</v>
       </c>
-      <c r="G99" s="94" t="s">
+      <c r="G99" s="95" t="s">
         <v>285</v>
       </c>
-      <c r="H99" s="94" t="s">
+      <c r="H99" s="95" t="s">
         <v>286</v>
       </c>
-      <c r="I99" s="94" t="s">
+      <c r="I99" s="95" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="100" spans="2:9">
       <c r="B100" s="8"/>
-      <c r="C100" s="94"/>
-      <c r="D100" s="94"/>
-      <c r="E100" s="94"/>
-      <c r="F100" s="94"/>
-      <c r="G100" s="94"/>
-      <c r="H100" s="94"/>
-      <c r="I100" s="94"/>
+      <c r="C100" s="95"/>
+      <c r="D100" s="95"/>
+      <c r="E100" s="95"/>
+      <c r="F100" s="95"/>
+      <c r="G100" s="95"/>
+      <c r="H100" s="95"/>
+      <c r="I100" s="95"/>
     </row>
     <row r="101" spans="2:9" ht="22.2" thickBot="1">
       <c r="B101" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C101" s="95"/>
-      <c r="D101" s="95"/>
-      <c r="E101" s="95"/>
-      <c r="F101" s="95"/>
-      <c r="G101" s="95"/>
-      <c r="H101" s="95"/>
-      <c r="I101" s="95"/>
+      <c r="C101" s="96"/>
+      <c r="D101" s="96"/>
+      <c r="E101" s="96"/>
+      <c r="F101" s="96"/>
+      <c r="G101" s="96"/>
+      <c r="H101" s="96"/>
+      <c r="I101" s="96"/>
     </row>
     <row r="102" spans="2:9" ht="75.599999999999994">
       <c r="B102" s="5" t="s">
@@ -10716,22 +10716,22 @@
       <c r="B154" s="11"/>
     </row>
     <row r="155" spans="2:5" ht="30.6" customHeight="1">
-      <c r="B155" s="97"/>
-      <c r="C155" s="99" t="s">
+      <c r="B155" s="98"/>
+      <c r="C155" s="100" t="s">
         <v>566</v>
       </c>
-      <c r="D155" s="94" t="s">
+      <c r="D155" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="E155" s="94" t="s">
+      <c r="E155" s="95" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="156" spans="2:5" ht="15" customHeight="1" thickBot="1">
-      <c r="B156" s="98"/>
-      <c r="C156" s="100"/>
-      <c r="D156" s="95"/>
-      <c r="E156" s="95"/>
+      <c r="B156" s="99"/>
+      <c r="C156" s="101"/>
+      <c r="D156" s="96"/>
+      <c r="E156" s="96"/>
     </row>
     <row r="157" spans="2:5">
       <c r="B157" s="5" t="s">
@@ -10777,22 +10777,22 @@
       <c r="B164" s="11"/>
     </row>
     <row r="165" spans="2:5">
-      <c r="B165" s="97"/>
-      <c r="C165" s="99" t="s">
+      <c r="B165" s="98"/>
+      <c r="C165" s="100" t="s">
         <v>567</v>
       </c>
-      <c r="D165" s="94" t="s">
+      <c r="D165" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="E165" s="94" t="s">
+      <c r="E165" s="95" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="166" spans="2:5" ht="44.4" customHeight="1" thickBot="1">
-      <c r="B166" s="98"/>
-      <c r="C166" s="100"/>
-      <c r="D166" s="95"/>
-      <c r="E166" s="95"/>
+      <c r="B166" s="99"/>
+      <c r="C166" s="101"/>
+      <c r="D166" s="96"/>
+      <c r="E166" s="96"/>
     </row>
     <row r="167" spans="2:5" ht="21.6">
       <c r="B167" s="5" t="s">
@@ -10838,22 +10838,22 @@
       <c r="B174" s="11"/>
     </row>
     <row r="175" spans="2:5" ht="20.399999999999999" customHeight="1">
-      <c r="B175" s="97"/>
-      <c r="C175" s="99" t="s">
+      <c r="B175" s="98"/>
+      <c r="C175" s="100" t="s">
         <v>568</v>
       </c>
-      <c r="D175" s="94" t="s">
+      <c r="D175" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="E175" s="94" t="s">
+      <c r="E175" s="95" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="176" spans="2:5" ht="21" customHeight="1" thickBot="1">
-      <c r="B176" s="98"/>
-      <c r="C176" s="100"/>
-      <c r="D176" s="95"/>
-      <c r="E176" s="95"/>
+      <c r="B176" s="99"/>
+      <c r="C176" s="101"/>
+      <c r="D176" s="96"/>
+      <c r="E176" s="96"/>
     </row>
     <row r="177" spans="2:6">
       <c r="B177" s="5" t="s">
@@ -11061,27 +11061,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="E155:E156"/>
-    <mergeCell ref="E165:E166"/>
-    <mergeCell ref="E175:E176"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="I99:I101"/>
-    <mergeCell ref="E99:E101"/>
-    <mergeCell ref="F99:F101"/>
-    <mergeCell ref="G99:G101"/>
-    <mergeCell ref="H99:H101"/>
-    <mergeCell ref="B165:B166"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="D165:D166"/>
-    <mergeCell ref="B175:B176"/>
-    <mergeCell ref="C175:C176"/>
-    <mergeCell ref="D175:D176"/>
-    <mergeCell ref="B155:B156"/>
-    <mergeCell ref="C155:C156"/>
-    <mergeCell ref="D155:D156"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="D99:D101"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
@@ -11098,6 +11077,27 @@
     <mergeCell ref="E29:E32"/>
     <mergeCell ref="F29:F32"/>
     <mergeCell ref="G29:G32"/>
+    <mergeCell ref="B155:B156"/>
+    <mergeCell ref="C155:C156"/>
+    <mergeCell ref="D155:D156"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="D99:D101"/>
+    <mergeCell ref="B165:B166"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="D165:D166"/>
+    <mergeCell ref="B175:B176"/>
+    <mergeCell ref="C175:C176"/>
+    <mergeCell ref="D175:D176"/>
+    <mergeCell ref="E155:E156"/>
+    <mergeCell ref="E165:E166"/>
+    <mergeCell ref="E175:E176"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="J29:J31"/>
+    <mergeCell ref="I99:I101"/>
+    <mergeCell ref="E99:E101"/>
+    <mergeCell ref="F99:F101"/>
+    <mergeCell ref="G99:G101"/>
+    <mergeCell ref="H99:H101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11163,13 +11163,13 @@
     </row>
     <row r="9" spans="2:7" ht="14.4">
       <c r="B9" s="4"/>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="95" t="s">
         <v>322</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="95" t="s">
         <v>323</v>
       </c>
-      <c r="E9" s="94" t="s">
+      <c r="E9" s="95" t="s">
         <v>324</v>
       </c>
       <c r="F9" s="2"/>
@@ -11177,10 +11177,10 @@
     </row>
     <row r="10" spans="2:7" ht="81.599999999999994" customHeight="1">
       <c r="B10" s="4"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94" t="s">
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95" t="s">
         <v>325</v>
       </c>
       <c r="G10"/>
@@ -11189,10 +11189,10 @@
       <c r="B11" s="79" t="s">
         <v>326</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
       <c r="G11"/>
     </row>
     <row r="12" spans="2:7" ht="14.4">
@@ -11436,48 +11436,48 @@
     </row>
     <row r="40" spans="2:9" ht="91.95" customHeight="1">
       <c r="B40" s="4"/>
-      <c r="C40" s="94" t="s">
+      <c r="C40" s="95" t="s">
         <v>338</v>
       </c>
-      <c r="D40" s="94" t="s">
+      <c r="D40" s="95" t="s">
         <v>339</v>
       </c>
-      <c r="E40" s="94" t="s">
+      <c r="E40" s="95" t="s">
         <v>340</v>
       </c>
-      <c r="F40" s="94" t="s">
+      <c r="F40" s="95" t="s">
         <v>341</v>
       </c>
-      <c r="G40" s="94" t="s">
+      <c r="G40" s="95" t="s">
         <v>342</v>
       </c>
-      <c r="H40" s="94" t="s">
+      <c r="H40" s="95" t="s">
         <v>343</v>
       </c>
-      <c r="I40" s="94" t="s">
+      <c r="I40" s="95" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="41" spans="2:9">
       <c r="B41" s="4"/>
-      <c r="C41" s="94"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="94"/>
-      <c r="G41" s="94"/>
-      <c r="H41" s="94"/>
-      <c r="I41" s="109"/>
+      <c r="C41" s="95"/>
+      <c r="D41" s="95"/>
+      <c r="E41" s="95"/>
+      <c r="F41" s="95"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="95"/>
+      <c r="I41" s="115"/>
     </row>
     <row r="42" spans="2:9" ht="11.4" thickBot="1">
       <c r="B42" s="79" t="s">
         <v>326</v>
       </c>
-      <c r="C42" s="95"/>
-      <c r="D42" s="95"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="95"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="95"/>
+      <c r="C42" s="96"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="96"/>
+      <c r="H42" s="96"/>
       <c r="I42" s="25"/>
     </row>
     <row r="43" spans="2:9">
@@ -13331,10 +13331,10 @@
       <c r="B265" s="11"/>
     </row>
     <row r="266" spans="2:6" ht="79.2" customHeight="1" thickBot="1">
-      <c r="B266" s="114" t="s">
+      <c r="B266" s="113" t="s">
         <v>430</v>
       </c>
-      <c r="C266" s="114"/>
+      <c r="C266" s="113"/>
       <c r="D266" s="1"/>
       <c r="E266" s="1" t="s">
         <v>304</v>
@@ -13344,10 +13344,10 @@
       </c>
     </row>
     <row r="267" spans="2:6">
-      <c r="B267" s="112" t="s">
+      <c r="B267" s="111" t="s">
         <v>431</v>
       </c>
-      <c r="C267" s="113"/>
+      <c r="C267" s="112"/>
       <c r="D267" s="6" t="s">
         <v>420</v>
       </c>
@@ -13447,10 +13447,10 @@
       </c>
     </row>
     <row r="274" spans="2:6" ht="40.200000000000003" customHeight="1">
-      <c r="B274" s="110" t="s">
+      <c r="B274" s="109" t="s">
         <v>438</v>
       </c>
-      <c r="C274" s="111"/>
+      <c r="C274" s="110"/>
       <c r="D274" s="6" t="s">
         <v>306</v>
       </c>
@@ -13462,19 +13462,19 @@
       </c>
     </row>
     <row r="275" spans="2:6" ht="12.6" customHeight="1" thickBot="1">
-      <c r="B275" s="115" t="s">
+      <c r="B275" s="114" t="s">
         <v>439</v>
       </c>
-      <c r="C275" s="115"/>
+      <c r="C275" s="114"/>
       <c r="D275" s="1"/>
       <c r="E275" s="1"/>
       <c r="F275" s="15"/>
     </row>
     <row r="276" spans="2:6">
-      <c r="B276" s="112" t="s">
+      <c r="B276" s="111" t="s">
         <v>431</v>
       </c>
-      <c r="C276" s="113"/>
+      <c r="C276" s="112"/>
       <c r="E276" s="6" t="s">
         <v>24</v>
       </c>
@@ -13573,10 +13573,10 @@
       </c>
     </row>
     <row r="283" spans="2:6" ht="40.200000000000003" customHeight="1">
-      <c r="B283" s="110" t="s">
+      <c r="B283" s="109" t="s">
         <v>438</v>
       </c>
-      <c r="C283" s="111"/>
+      <c r="C283" s="110"/>
       <c r="D283" s="6" t="s">
         <v>306</v>
       </c>
@@ -14304,6 +14304,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
     <mergeCell ref="B283:C283"/>
     <mergeCell ref="B276:C276"/>
     <mergeCell ref="B267:C267"/>
@@ -14316,11 +14321,6 @@
     <mergeCell ref="G40:G42"/>
     <mergeCell ref="B266:C266"/>
     <mergeCell ref="B275:C275"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14333,21 +14333,21 @@
   <dimension ref="A1:U64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="4.88671875" style="90" customWidth="1"/>
     <col min="2" max="3" width="42.44140625" style="90" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="90" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="90" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="90" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" style="90" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" style="90" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="90" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="90" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="90" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" style="90" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" style="90" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" style="90" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.33203125" style="90" customWidth="1"/>
     <col min="11" max="11" width="23.109375" style="90" customWidth="1"/>
@@ -17493,43 +17493,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e9cfd4ee-a8d7-4822-bab8-2f7341ccf5f7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b13c4baf-4ec4-4575-9704-16f8abed6659">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="e9cfd4ee-a8d7-4822-bab8-2f7341ccf5f7">
-      <UserInfo>
-        <DisplayName>Olivier Gil</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Alice Tan</DisplayName>
-        <AccountId>211</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Anne-Sophie SIX</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FBB7BE0DBFEBA4E9AF4097A6101E116" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0019dcb484b721c90a55a8aa2b1809bd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b13c4baf-4ec4-4575-9704-16f8abed6659" xmlns:ns3="e9cfd4ee-a8d7-4822-bab8-2f7341ccf5f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68dae707afab8505bf60de61140799b9" ns2:_="" ns3:_="">
     <xsd:import namespace="b13c4baf-4ec4-4575-9704-16f8abed6659"/>
@@ -17778,32 +17741,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{736D09C3-EB7E-458E-963D-BA7CB31D47CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e9cfd4ee-a8d7-4822-bab8-2f7341ccf5f7"/>
-    <ds:schemaRef ds:uri="b13c4baf-4ec4-4575-9704-16f8abed6659"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E4AEF6D-231D-428A-96EF-68C4A91FA8B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e9cfd4ee-a8d7-4822-bab8-2f7341ccf5f7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b13c4baf-4ec4-4575-9704-16f8abed6659">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="e9cfd4ee-a8d7-4822-bab8-2f7341ccf5f7">
+      <UserInfo>
+        <DisplayName>Olivier Gil</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Alice Tan</DisplayName>
+        <AccountId>211</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Anne-Sophie SIX</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DDFCFF7-1DBA-48B6-853E-FE1828FA4029}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17820,4 +17795,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E4AEF6D-231D-428A-96EF-68C4A91FA8B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{736D09C3-EB7E-458E-963D-BA7CB31D47CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e9cfd4ee-a8d7-4822-bab8-2f7341ccf5f7"/>
+    <ds:schemaRef ds:uri="b13c4baf-4ec4-4575-9704-16f8abed6659"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>